<commit_message>
D1, D2 , D3, D4
</commit_message>
<xml_diff>
--- a/tablaExamenPilotp2011v1.xlsx
+++ b/tablaExamenPilotp2011v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="23">
   <si>
     <t>A</t>
   </si>
@@ -120,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,6 +570,17 @@
     <tableColumn id="3" name="Respuestas"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="F2:G46" totalsRowShown="0">
+  <autoFilter ref="F2:G46"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="D"/>
+    <tableColumn id="2" name="Respuestas"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -859,19 +871,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="6" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -881,8 +894,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1.1000000000000001</v>
       </c>
@@ -892,16 +911,25 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.2</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.3</v>
       </c>
@@ -911,40 +939,64 @@
       <c r="D5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.4</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.5</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.6</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.7</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0.7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.8</v>
       </c>
@@ -954,8 +1006,14 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1.9</v>
       </c>
@@ -965,8 +1023,14 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0.9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -976,24 +1040,36 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.1100000000000001</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.1200000000000001</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.1299999999999999</v>
       </c>
@@ -1003,16 +1079,28 @@
       <c r="D15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1.1399999999999999</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>0.2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1.1499999999999999</v>
       </c>
@@ -1022,133 +1110,336 @@
       <c r="D17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>0.6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>0.7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>0.8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>0.9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>0.2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>18</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>0.3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>19</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>0.4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>20</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>21</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>0.6</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>22</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
+      </c>
+      <c r="F32">
+        <v>0.7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>0.8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>0.9</v>
+      </c>
+      <c r="G34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>0.1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>0.2</v>
+      </c>
+      <c r="G38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>0.3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>0.4</v>
+      </c>
+      <c r="G40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>0.5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>0.6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>0.7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>0.8</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>0.9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>